<commit_message>
1DES SOP excel aula08
</commit_message>
<xml_diff>
--- a/1des/sop/aula09/FolhaDePag.xlsx
+++ b/1des/sop/aula09/FolhaDePag.xlsx
@@ -471,7 +471,7 @@
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -569,15 +569,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,6 +579,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -876,7 +876,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,20 +892,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="B1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="15"/>
+      <c r="H1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -926,7 +926,7 @@
       <c r="I2" s="3">
         <v>1100.01</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="9">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
@@ -1038,12 +1038,12 @@
       <c r="B9" s="3">
         <v>1558.5</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1058,7 +1058,7 @@
       <c r="I10" s="3">
         <v>0</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="9">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
@@ -1134,25 +1134,25 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="12"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="10"/>
     </row>
     <row r="17" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
         <v>79</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="10" t="s">
         <v>80</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L17" s="12"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
@@ -1175,7 +1175,7 @@
       <c r="I19" s="3">
         <v>1903.99</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="9">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="K19" s="3">
@@ -1189,7 +1189,7 @@
       <c r="I20" s="3">
         <v>2826.66</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="9">
         <v>0.15</v>
       </c>
       <c r="K20" s="3">
@@ -1204,7 +1204,7 @@
       <c r="I21" s="3">
         <v>3751.06</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="9">
         <v>0.22500000000000001</v>
       </c>
       <c r="K21" s="3">
@@ -1218,7 +1218,7 @@
       <c r="I22" s="3">
         <v>4664.68</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="9">
         <v>0.27500000000000002</v>
       </c>
       <c r="K22" s="3">
@@ -1251,8 +1251,8 @@
   <sheetPr codeName="Plan2"/>
   <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,10 +1300,10 @@
       <c r="S1" s="17"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
@@ -1331,66 +1331,66 @@
       <c r="H5" s="2">
         <v>0.5</v>
       </c>
-      <c r="S5" s="16">
+      <c r="S5" s="14">
         <v>0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="R6" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="12" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1433,24 +1433,24 @@
         <f ca="1">F7+I7+J7</f>
         <v>2078</v>
       </c>
-      <c r="L7" s="13">
-        <f ca="1">VLOOKUP(K7,inss,2)</f>
+      <c r="L7" s="11">
+        <f t="shared" ref="L7:L43" ca="1" si="0">VLOOKUP(K7,inss,2)</f>
         <v>0.09</v>
       </c>
       <c r="M7" s="5">
-        <f ca="1">IF(L7="Teto",900.7,F7*L7)</f>
+        <f t="shared" ref="M7:M43" ca="1" si="1">IF(L7="Teto",900.7,F7*L7)</f>
         <v>187.01999999999998</v>
       </c>
       <c r="N7" s="5">
         <f ca="1">K7-M7</f>
         <v>1890.98</v>
       </c>
-      <c r="O7" s="13" t="str">
-        <f ca="1">VLOOKUP(N7,irrf,2)</f>
+      <c r="O7" s="11" t="str">
+        <f t="shared" ref="O7:O43" ca="1" si="2">VLOOKUP(N7,irrf,2)</f>
         <v>isento</v>
       </c>
       <c r="P7" s="3">
-        <f ca="1">VLOOKUP(N7,irrf,3)</f>
+        <f t="shared" ref="P7:P43" ca="1" si="3">VLOOKUP(N7,irrf,3)</f>
         <v>0</v>
       </c>
       <c r="Q7" s="5">
@@ -1480,61 +1480,61 @@
         <v>43</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f t="shared" ref="E8:E43" ca="1" si="0">IF(TRUNC((TODAY()-C8)/365)&lt;1,$E$3,IF(TRUNC((TODAY()-C8)/365)&lt;3,$E$4,$E$5))</f>
+        <f t="shared" ref="E8:E43" ca="1" si="4">IF(TRUNC((TODAY()-C8)/365)&lt;1,$E$3,IF(TRUNC((TODAY()-C8)/365)&lt;3,$E$4,$E$5))</f>
         <v>Pleno</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" ref="F7:F43" ca="1" si="1">VLOOKUP(D8,cargos,2)+VLOOKUP(D8,cargos,2)*VLOOKUP(E8,carreira,2)</f>
+        <f t="shared" ref="F8:F43" ca="1" si="5">VLOOKUP(D8,cargos,2)+VLOOKUP(D8,cargos,2)*VLOOKUP(E8,carreira,2)</f>
         <v>2026.05</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" ref="G8:G43" ca="1" si="2">F8/220</f>
+        <f t="shared" ref="G8:G43" ca="1" si="6">F8/220</f>
         <v>9.2093181818181815</v>
       </c>
       <c r="H8">
         <v>2</v>
       </c>
       <c r="I8" s="3">
-        <f t="shared" ref="I8:I43" ca="1" si="3">(G8+G8*$H$5)*H8</f>
+        <f t="shared" ref="I8:I43" ca="1" si="7">(G8+G8*$H$5)*H8</f>
         <v>27.627954545454543</v>
       </c>
       <c r="J8" s="3">
         <v>0</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" ref="K8:K43" ca="1" si="4">F8+I8+J8</f>
+        <f t="shared" ref="K8:K43" ca="1" si="8">F8+I8+J8</f>
         <v>2053.6779545454547</v>
       </c>
-      <c r="L8" s="13">
-        <f ca="1">VLOOKUP(K8,inss,2)</f>
+      <c r="L8" s="11">
+        <f t="shared" ca="1" si="0"/>
         <v>0.09</v>
       </c>
       <c r="M8" s="5">
-        <f ca="1">IF(L8="Teto",900.7,F8*L8)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>182.34449999999998</v>
       </c>
       <c r="N8" s="5">
-        <f t="shared" ref="N8:N43" ca="1" si="5">K8-M8</f>
+        <f t="shared" ref="N8:N43" ca="1" si="9">K8-M8</f>
         <v>1871.3334545454547</v>
       </c>
-      <c r="O8" s="13" t="str">
-        <f ca="1">VLOOKUP(N8,irrf,2)</f>
+      <c r="O8" s="11" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>isento</v>
       </c>
       <c r="P8" s="3">
-        <f ca="1">VLOOKUP(N8,irrf,3)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="Q8" s="5">
-        <f t="shared" ref="Q8" ca="1" si="6">IF(O8="isento",0,N8*O8-P8)</f>
+        <f t="shared" ref="Q8" ca="1" si="10">IF(O8="isento",0,N8*O8-P8)</f>
         <v>0</v>
       </c>
       <c r="R8" s="5">
-        <f t="shared" ref="R8:R43" ca="1" si="7">N8-Q8</f>
+        <f t="shared" ref="R8:R43" ca="1" si="11">N8-Q8</f>
         <v>1871.3334545454547</v>
       </c>
       <c r="S8" s="5">
-        <f t="shared" ref="S8:S43" ca="1" si="8">N8*8%</f>
+        <f t="shared" ref="S8:S43" ca="1" si="12">N8*8%</f>
         <v>149.70667636363638</v>
       </c>
     </row>
@@ -1552,49 +1552,49 @@
         <v>49</v>
       </c>
       <c r="E9" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Pleno</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2431.2600000000002</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>11.051181818181819</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2431.2600000000002</v>
+      </c>
+      <c r="L9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Pleno</v>
-      </c>
-      <c r="F9" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M9" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2431.2600000000002</v>
-      </c>
-      <c r="G9" s="3">
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N9" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2139.5088000000001</v>
+      </c>
+      <c r="O9" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>11.051181818181819</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P9" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2431.2600000000002</v>
-      </c>
-      <c r="L9" s="13">
-        <f ca="1">VLOOKUP(K9,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M9" s="5">
-        <f ca="1">IF(L9="Teto",900.7,F9*L9)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N9" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2139.5088000000001</v>
-      </c>
-      <c r="O9" s="13">
-        <f ca="1">VLOOKUP(N9,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P9" s="3">
-        <f ca="1">VLOOKUP(N9,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q9" s="5">
@@ -1602,11 +1602,11 @@
         <v>17.663159999999976</v>
       </c>
       <c r="R9" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2121.84564</v>
       </c>
       <c r="S9" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>171.16070400000001</v>
       </c>
     </row>
@@ -1624,61 +1624,61 @@
         <v>44</v>
       </c>
       <c r="E10" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2431.2600000000002</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>11.051181818181819</v>
       </c>
       <c r="H10">
         <v>15</v>
       </c>
       <c r="I10" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>248.65159090909094</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2679.911590909091</v>
+      </c>
+      <c r="L10" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="M10" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N10" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2388.1603909090909</v>
+      </c>
+      <c r="O10" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P10" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>248.65159090909094</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2679.911590909091</v>
-      </c>
-      <c r="L10" s="13">
-        <f ca="1">VLOOKUP(K10,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M10" s="5">
-        <f ca="1">IF(L10="Teto",900.7,F10*L10)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N10" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2388.1603909090909</v>
-      </c>
-      <c r="O10" s="13">
-        <f ca="1">VLOOKUP(N10,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P10" s="3">
-        <f ca="1">VLOOKUP(N10,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q10" s="5">
-        <f t="shared" ref="Q10:Q43" ca="1" si="9">IF(O10="isento",0,N10*O10-P10)</f>
+        <f t="shared" ref="Q10:Q43" ca="1" si="13">IF(O10="isento",0,N10*O10-P10)</f>
         <v>36.3120293181818</v>
       </c>
       <c r="R10" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2351.848361590909</v>
       </c>
       <c r="S10" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>191.05283127272727</v>
       </c>
     </row>
@@ -1696,61 +1696,61 @@
         <v>67</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>7800</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>35.454545454545453</v>
       </c>
       <c r="H11">
         <v>12</v>
       </c>
       <c r="I11" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>638.18181818181813</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>8438.181818181818</v>
+      </c>
+      <c r="L11" s="11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Teto</v>
+      </c>
+      <c r="M11" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>900.7</v>
+      </c>
+      <c r="N11" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>7537.4818181818182</v>
+      </c>
+      <c r="O11" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="P11" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>638.18181818181813</v>
-      </c>
-      <c r="J11" s="3">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>8438.181818181818</v>
-      </c>
-      <c r="L11" s="13" t="str">
-        <f ca="1">VLOOKUP(K11,inss,2)</f>
-        <v>Teto</v>
-      </c>
-      <c r="M11" s="5">
-        <f ca="1">IF(L11="Teto",900.7,F11*L11)</f>
-        <v>900.7</v>
-      </c>
-      <c r="N11" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>7537.4818181818182</v>
-      </c>
-      <c r="O11" s="13">
-        <f ca="1">VLOOKUP(N11,irrf,2)</f>
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="P11" s="3">
-        <f ca="1">VLOOKUP(N11,irrf,3)</f>
         <v>869.36</v>
       </c>
       <c r="Q11" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>1203.4475000000002</v>
       </c>
       <c r="R11" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6334.034318181818</v>
       </c>
       <c r="S11" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>602.99854545454548</v>
       </c>
     </row>
@@ -1768,61 +1768,61 @@
         <v>48</v>
       </c>
       <c r="E12" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2701.4</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>12.279090909090909</v>
       </c>
       <c r="H12">
         <v>8</v>
       </c>
       <c r="I12" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>147.3490909090909</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2848.7490909090911</v>
+      </c>
+      <c r="L12" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>324.16800000000001</v>
+      </c>
+      <c r="N12" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2524.581090909091</v>
+      </c>
+      <c r="O12" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P12" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>147.3490909090909</v>
-      </c>
-      <c r="J12" s="3">
-        <v>0</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2848.7490909090911</v>
-      </c>
-      <c r="L12" s="13">
-        <f ca="1">VLOOKUP(K12,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M12" s="5">
-        <f ca="1">IF(L12="Teto",900.7,F12*L12)</f>
-        <v>324.16800000000001</v>
-      </c>
-      <c r="N12" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2524.581090909091</v>
-      </c>
-      <c r="O12" s="13">
-        <f ca="1">VLOOKUP(N12,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P12" s="3">
-        <f ca="1">VLOOKUP(N12,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q12" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>46.543581818181821</v>
       </c>
       <c r="R12" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2478.0375090909092</v>
       </c>
       <c r="S12" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>201.96648727272728</v>
       </c>
     </row>
@@ -1840,61 +1840,61 @@
         <v>47</v>
       </c>
       <c r="E13" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Senior</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2992.3199999999997</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>13.601454545454544</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2992.3199999999997</v>
+      </c>
+      <c r="L13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Senior</v>
-      </c>
-      <c r="F13" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M13" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2992.3199999999997</v>
-      </c>
-      <c r="G13" s="3">
+        <v>359.07839999999993</v>
+      </c>
+      <c r="N13" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2633.2415999999998</v>
+      </c>
+      <c r="O13" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>13.601454545454544</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P13" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2992.3199999999997</v>
-      </c>
-      <c r="L13" s="13">
-        <f ca="1">VLOOKUP(K13,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M13" s="5">
-        <f ca="1">IF(L13="Teto",900.7,F13*L13)</f>
-        <v>359.07839999999993</v>
-      </c>
-      <c r="N13" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2633.2415999999998</v>
-      </c>
-      <c r="O13" s="13">
-        <f ca="1">VLOOKUP(N13,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P13" s="3">
-        <f ca="1">VLOOKUP(N13,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q13" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>54.693119999999965</v>
       </c>
       <c r="R13" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2578.5484799999999</v>
       </c>
       <c r="S13" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>210.65932799999999</v>
       </c>
     </row>
@@ -1912,61 +1912,61 @@
         <v>77</v>
       </c>
       <c r="E14" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Júnior</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1039</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>4.7227272727272727</v>
       </c>
       <c r="H14">
         <v>7</v>
       </c>
       <c r="I14" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>49.588636363636361</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>1088.5886363636364</v>
+      </c>
+      <c r="L14" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>77.924999999999997</v>
+      </c>
+      <c r="N14" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>1010.6636363636364</v>
+      </c>
+      <c r="O14" s="11" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>isento</v>
+      </c>
+      <c r="P14" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>49.588636363636361</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0</v>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>1088.5886363636364</v>
-      </c>
-      <c r="L14" s="13">
-        <f ca="1">VLOOKUP(K14,inss,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="M14" s="5">
-        <f ca="1">IF(L14="Teto",900.7,F14*L14)</f>
-        <v>77.924999999999997</v>
-      </c>
-      <c r="N14" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="5">
+        <f t="shared" ca="1" si="11"/>
         <v>1010.6636363636364</v>
       </c>
-      <c r="O14" s="13" t="str">
-        <f ca="1">VLOOKUP(N14,irrf,2)</f>
-        <v>isento</v>
-      </c>
-      <c r="P14" s="3">
-        <f ca="1">VLOOKUP(N14,irrf,3)</f>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="5">
-        <f t="shared" ca="1" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="5">
-        <f t="shared" ca="1" si="7"/>
-        <v>1010.6636363636364</v>
-      </c>
       <c r="S14" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>80.853090909090923</v>
       </c>
     </row>
@@ -1984,61 +1984,61 @@
         <v>42</v>
       </c>
       <c r="E15" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>3376.75</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>15.348863636363637</v>
       </c>
       <c r="H15">
         <v>9</v>
       </c>
       <c r="I15" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>207.2096590909091</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>3583.9596590909091</v>
+      </c>
+      <c r="L15" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M15" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>472.74500000000006</v>
+      </c>
+      <c r="N15" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>3111.2146590909092</v>
+      </c>
+      <c r="O15" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="P15" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>207.2096590909091</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0</v>
-      </c>
-      <c r="K15" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3583.9596590909091</v>
-      </c>
-      <c r="L15" s="13">
-        <f ca="1">VLOOKUP(K15,inss,2)</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M15" s="5">
-        <f ca="1">IF(L15="Teto",900.7,F15*L15)</f>
-        <v>472.74500000000006</v>
-      </c>
-      <c r="N15" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>3111.2146590909092</v>
-      </c>
-      <c r="O15" s="13">
-        <f ca="1">VLOOKUP(N15,irrf,2)</f>
-        <v>0.15</v>
-      </c>
-      <c r="P15" s="3">
-        <f ca="1">VLOOKUP(N15,irrf,3)</f>
         <v>354.8</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>111.88219886363635</v>
       </c>
       <c r="R15" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2999.3324602272728</v>
       </c>
       <c r="S15" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>248.89717272727273</v>
       </c>
     </row>
@@ -2056,61 +2056,61 @@
         <v>46</v>
       </c>
       <c r="E16" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2431.2600000000002</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>11.051181818181819</v>
       </c>
       <c r="H16">
         <v>6</v>
       </c>
       <c r="I16" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="7"/>
         <v>99.460636363636382</v>
       </c>
       <c r="J16" s="3">
         <v>200</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="8"/>
         <v>2730.7206363636365</v>
       </c>
-      <c r="L16" s="13">
-        <f ca="1">VLOOKUP(K16,inss,2)</f>
+      <c r="L16" s="11">
+        <f t="shared" ca="1" si="0"/>
         <v>0.12</v>
       </c>
       <c r="M16" s="5">
-        <f ca="1">IF(L16="Teto",900.7,F16*L16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>291.75120000000004</v>
       </c>
       <c r="N16" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="9"/>
         <v>2438.9694363636363</v>
       </c>
-      <c r="O16" s="13">
-        <f ca="1">VLOOKUP(N16,irrf,2)</f>
+      <c r="O16" s="11">
+        <f t="shared" ca="1" si="2"/>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="P16" s="3">
-        <f ca="1">VLOOKUP(N16,irrf,3)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>142.80000000000001</v>
       </c>
       <c r="Q16" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>40.122707727272712</v>
       </c>
       <c r="R16" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2398.8467286363634</v>
       </c>
       <c r="S16" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>195.1175549090909</v>
       </c>
     </row>
@@ -2128,61 +2128,61 @@
         <v>46</v>
       </c>
       <c r="E17" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2431.2600000000002</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>11.051181818181819</v>
       </c>
       <c r="H17">
         <v>12</v>
       </c>
       <c r="I17" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>198.92127272727276</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2630.1812727272732</v>
+      </c>
+      <c r="L17" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N17" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2338.430072727273</v>
+      </c>
+      <c r="O17" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P17" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>198.92127272727276</v>
-      </c>
-      <c r="J17" s="3">
-        <v>0</v>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2630.1812727272732</v>
-      </c>
-      <c r="L17" s="13">
-        <f ca="1">VLOOKUP(K17,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M17" s="5">
-        <f ca="1">IF(L17="Teto",900.7,F17*L17)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N17" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2338.430072727273</v>
-      </c>
-      <c r="O17" s="13">
-        <f ca="1">VLOOKUP(N17,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P17" s="3">
-        <f ca="1">VLOOKUP(N17,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q17" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>32.582255454545447</v>
       </c>
       <c r="R17" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2305.8478172727278</v>
       </c>
       <c r="S17" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>187.07440581818184</v>
       </c>
     </row>
@@ -2200,61 +2200,61 @@
         <v>45</v>
       </c>
       <c r="E18" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Pleno</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2701.4</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>12.279090909090909</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2701.4</v>
+      </c>
+      <c r="L18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Pleno</v>
-      </c>
-      <c r="F18" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M18" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2701.4</v>
-      </c>
-      <c r="G18" s="3">
+        <v>324.16800000000001</v>
+      </c>
+      <c r="N18" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2377.232</v>
+      </c>
+      <c r="O18" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>12.279090909090909</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P18" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0</v>
-      </c>
-      <c r="K18" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2701.4</v>
-      </c>
-      <c r="L18" s="13">
-        <f ca="1">VLOOKUP(K18,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M18" s="5">
-        <f ca="1">IF(L18="Teto",900.7,F18*L18)</f>
-        <v>324.16800000000001</v>
-      </c>
-      <c r="N18" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2377.232</v>
-      </c>
-      <c r="O18" s="13">
-        <f ca="1">VLOOKUP(N18,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P18" s="3">
-        <f ca="1">VLOOKUP(N18,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q18" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>35.492399999999975</v>
       </c>
       <c r="R18" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2341.7395999999999</v>
       </c>
       <c r="S18" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>190.17856</v>
       </c>
     </row>
@@ -2272,61 +2272,61 @@
         <v>42</v>
       </c>
       <c r="E19" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Senior</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>4156</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>18.890909090909091</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>4156</v>
+      </c>
+      <c r="L19" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Senior</v>
-      </c>
-      <c r="F19" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M19" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>4156</v>
-      </c>
-      <c r="G19" s="3">
+        <v>581.84</v>
+      </c>
+      <c r="N19" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>3574.16</v>
+      </c>
+      <c r="O19" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>18.890909090909091</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="P19" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="3">
-        <v>0</v>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>4156</v>
-      </c>
-      <c r="L19" s="13">
-        <f ca="1">VLOOKUP(K19,inss,2)</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M19" s="5">
-        <f ca="1">IF(L19="Teto",900.7,F19*L19)</f>
-        <v>581.84</v>
-      </c>
-      <c r="N19" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>3574.16</v>
-      </c>
-      <c r="O19" s="13">
-        <f ca="1">VLOOKUP(N19,irrf,2)</f>
-        <v>0.15</v>
-      </c>
-      <c r="P19" s="3">
-        <f ca="1">VLOOKUP(N19,irrf,3)</f>
         <v>354.8</v>
       </c>
       <c r="Q19" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>181.3239999999999</v>
       </c>
       <c r="R19" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>3392.8359999999998</v>
       </c>
       <c r="S19" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>285.93279999999999</v>
       </c>
     </row>
@@ -2344,61 +2344,61 @@
         <v>47</v>
       </c>
       <c r="E20" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2431.2600000000002</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>11.051181818181819</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="I20" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>16.576772727272729</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2447.836772727273</v>
+      </c>
+      <c r="L20" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="M20" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N20" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2156.0855727272728</v>
+      </c>
+      <c r="O20" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P20" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>16.576772727272729</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0</v>
-      </c>
-      <c r="K20" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2447.836772727273</v>
-      </c>
-      <c r="L20" s="13">
-        <f ca="1">VLOOKUP(K20,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M20" s="5">
-        <f ca="1">IF(L20="Teto",900.7,F20*L20)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N20" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2156.0855727272728</v>
-      </c>
-      <c r="O20" s="13">
-        <f ca="1">VLOOKUP(N20,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P20" s="3">
-        <f ca="1">VLOOKUP(N20,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q20" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>18.906417954545446</v>
       </c>
       <c r="R20" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2137.1791547727275</v>
       </c>
       <c r="S20" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>172.48684581818182</v>
       </c>
     </row>
@@ -2416,61 +2416,61 @@
         <v>50</v>
       </c>
       <c r="E21" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Júnior</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>1870.2</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>8.5009090909090919</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>1870.2</v>
+      </c>
+      <c r="L21" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Júnior</v>
-      </c>
-      <c r="F21" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="M21" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>1870.2</v>
-      </c>
-      <c r="G21" s="3">
+        <v>168.31800000000001</v>
+      </c>
+      <c r="N21" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>1701.8820000000001</v>
+      </c>
+      <c r="O21" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>8.5009090909090919</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3">
+        <v>isento</v>
+      </c>
+      <c r="P21" s="3">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="3">
-        <v>0</v>
-      </c>
-      <c r="K21" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>1870.2</v>
-      </c>
-      <c r="L21" s="13">
-        <f ca="1">VLOOKUP(K21,inss,2)</f>
-        <v>0.09</v>
-      </c>
-      <c r="M21" s="5">
-        <f ca="1">IF(L21="Teto",900.7,F21*L21)</f>
-        <v>168.31800000000001</v>
-      </c>
-      <c r="N21" s="5">
-        <f t="shared" ca="1" si="5"/>
+      <c r="Q21" s="5">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="5">
+        <f t="shared" ca="1" si="11"/>
         <v>1701.8820000000001</v>
       </c>
-      <c r="O21" s="13" t="str">
-        <f ca="1">VLOOKUP(N21,irrf,2)</f>
-        <v>isento</v>
-      </c>
-      <c r="P21" s="3">
-        <f ca="1">VLOOKUP(N21,irrf,3)</f>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="5">
-        <f t="shared" ca="1" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="5">
-        <f t="shared" ca="1" si="7"/>
-        <v>1701.8820000000001</v>
-      </c>
       <c r="S21" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>136.15056000000001</v>
       </c>
     </row>
@@ -2488,61 +2488,61 @@
         <v>49</v>
       </c>
       <c r="E22" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2431.2600000000002</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>11.051181818181819</v>
       </c>
       <c r="H22">
         <v>2</v>
       </c>
       <c r="I22" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>33.153545454545458</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2464.4135454545458</v>
+      </c>
+      <c r="L22" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N22" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2172.6623454545456</v>
+      </c>
+      <c r="O22" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P22" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>33.153545454545458</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0</v>
-      </c>
-      <c r="K22" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2464.4135454545458</v>
-      </c>
-      <c r="L22" s="13">
-        <f ca="1">VLOOKUP(K22,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M22" s="5">
-        <f ca="1">IF(L22="Teto",900.7,F22*L22)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N22" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2172.6623454545456</v>
-      </c>
-      <c r="O22" s="13">
-        <f ca="1">VLOOKUP(N22,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P22" s="3">
-        <f ca="1">VLOOKUP(N22,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q22" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>20.149675909090917</v>
       </c>
       <c r="R22" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2152.5126695454546</v>
       </c>
       <c r="S22" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>173.81298763636366</v>
       </c>
     </row>
@@ -2560,61 +2560,61 @@
         <v>43</v>
       </c>
       <c r="E23" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2026.05</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>9.2093181818181815</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="7"/>
         <v>138.13977272727271</v>
       </c>
       <c r="J23" s="3">
         <v>500</v>
       </c>
       <c r="K23" s="3">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="8"/>
         <v>2664.1897727272726</v>
       </c>
-      <c r="L23" s="13">
-        <f ca="1">VLOOKUP(K23,inss,2)</f>
+      <c r="L23" s="11">
+        <f t="shared" ca="1" si="0"/>
         <v>0.12</v>
       </c>
       <c r="M23" s="5">
-        <f ca="1">IF(L23="Teto",900.7,F23*L23)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>243.12599999999998</v>
       </c>
       <c r="N23" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="9"/>
         <v>2421.0637727272724</v>
       </c>
-      <c r="O23" s="13">
-        <f ca="1">VLOOKUP(N23,irrf,2)</f>
+      <c r="O23" s="11">
+        <f t="shared" ca="1" si="2"/>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="P23" s="3">
-        <f ca="1">VLOOKUP(N23,irrf,3)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>142.80000000000001</v>
       </c>
       <c r="Q23" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>38.779782954545425</v>
       </c>
       <c r="R23" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2382.2839897727272</v>
       </c>
       <c r="S23" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>193.68510181818181</v>
       </c>
     </row>
@@ -2632,61 +2632,61 @@
         <v>43</v>
       </c>
       <c r="E24" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2026.05</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>9.2093181818181815</v>
       </c>
       <c r="H24">
         <v>3</v>
       </c>
       <c r="I24" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>41.441931818181814</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2067.4919318181819</v>
+      </c>
+      <c r="L24" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="M24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>182.34449999999998</v>
+      </c>
+      <c r="N24" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>1885.147431818182</v>
+      </c>
+      <c r="O24" s="11" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>isento</v>
+      </c>
+      <c r="P24" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>41.441931818181814</v>
-      </c>
-      <c r="J24" s="3">
-        <v>0</v>
-      </c>
-      <c r="K24" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2067.4919318181819</v>
-      </c>
-      <c r="L24" s="13">
-        <f ca="1">VLOOKUP(K24,inss,2)</f>
-        <v>0.09</v>
-      </c>
-      <c r="M24" s="5">
-        <f ca="1">IF(L24="Teto",900.7,F24*L24)</f>
-        <v>182.34449999999998</v>
-      </c>
-      <c r="N24" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="5">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="5">
+        <f t="shared" ca="1" si="11"/>
         <v>1885.147431818182</v>
       </c>
-      <c r="O24" s="13" t="str">
-        <f ca="1">VLOOKUP(N24,irrf,2)</f>
-        <v>isento</v>
-      </c>
-      <c r="P24" s="3">
-        <f ca="1">VLOOKUP(N24,irrf,3)</f>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="5">
-        <f t="shared" ca="1" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="5">
-        <f t="shared" ca="1" si="7"/>
-        <v>1885.147431818182</v>
-      </c>
       <c r="S24" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>150.81179454545457</v>
       </c>
     </row>
@@ -2704,61 +2704,61 @@
         <v>50</v>
       </c>
       <c r="E25" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Pleno</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2431.2600000000002</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>11.051181818181819</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2431.2600000000002</v>
+      </c>
+      <c r="L25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Pleno</v>
-      </c>
-      <c r="F25" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M25" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2431.2600000000002</v>
-      </c>
-      <c r="G25" s="3">
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N25" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2139.5088000000001</v>
+      </c>
+      <c r="O25" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>11.051181818181819</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P25" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="3">
-        <v>0</v>
-      </c>
-      <c r="K25" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2431.2600000000002</v>
-      </c>
-      <c r="L25" s="13">
-        <f ca="1">VLOOKUP(K25,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M25" s="5">
-        <f ca="1">IF(L25="Teto",900.7,F25*L25)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N25" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2139.5088000000001</v>
-      </c>
-      <c r="O25" s="13">
-        <f ca="1">VLOOKUP(N25,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P25" s="3">
-        <f ca="1">VLOOKUP(N25,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q25" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>17.663159999999976</v>
       </c>
       <c r="R25" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2121.84564</v>
       </c>
       <c r="S25" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>171.16070400000001</v>
       </c>
     </row>
@@ -2776,61 +2776,61 @@
         <v>49</v>
       </c>
       <c r="E26" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Senior</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2992.3199999999997</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>13.601454545454544</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
       <c r="I26" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>20.402181818181816</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>3012.7221818181815</v>
+      </c>
+      <c r="L26" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="M26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>359.07839999999993</v>
+      </c>
+      <c r="N26" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2653.6437818181817</v>
+      </c>
+      <c r="O26" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P26" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>20.402181818181816</v>
-      </c>
-      <c r="J26" s="3">
-        <v>0</v>
-      </c>
-      <c r="K26" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3012.7221818181815</v>
-      </c>
-      <c r="L26" s="13">
-        <f ca="1">VLOOKUP(K26,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M26" s="5">
-        <f ca="1">IF(L26="Teto",900.7,F26*L26)</f>
-        <v>359.07839999999993</v>
-      </c>
-      <c r="N26" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2653.6437818181817</v>
-      </c>
-      <c r="O26" s="13">
-        <f ca="1">VLOOKUP(N26,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P26" s="3">
-        <f ca="1">VLOOKUP(N26,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q26" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>56.223283636363618</v>
       </c>
       <c r="R26" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2597.4204981818179</v>
       </c>
       <c r="S26" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>212.29150254545453</v>
       </c>
     </row>
@@ -2848,61 +2848,61 @@
         <v>43</v>
       </c>
       <c r="E27" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Senior</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2493.6</v>
+      </c>
+      <c r="G27" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>11.334545454545454</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2493.6</v>
+      </c>
+      <c r="L27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Senior</v>
-      </c>
-      <c r="F27" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M27" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2493.6</v>
-      </c>
-      <c r="G27" s="3">
+        <v>299.23199999999997</v>
+      </c>
+      <c r="N27" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2194.3679999999999</v>
+      </c>
+      <c r="O27" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>11.334545454545454</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P27" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="3">
-        <v>0</v>
-      </c>
-      <c r="K27" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2493.6</v>
-      </c>
-      <c r="L27" s="13">
-        <f ca="1">VLOOKUP(K27,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M27" s="5">
-        <f ca="1">IF(L27="Teto",900.7,F27*L27)</f>
-        <v>299.23199999999997</v>
-      </c>
-      <c r="N27" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2194.3679999999999</v>
-      </c>
-      <c r="O27" s="13">
-        <f ca="1">VLOOKUP(N27,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P27" s="3">
-        <f ca="1">VLOOKUP(N27,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q27" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>21.777599999999978</v>
       </c>
       <c r="R27" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2172.5904</v>
       </c>
       <c r="S27" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>175.54944</v>
       </c>
     </row>
@@ -2920,61 +2920,61 @@
         <v>50</v>
       </c>
       <c r="E28" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Júnior</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>1870.2</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>8.5009090909090919</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>1870.2</v>
+      </c>
+      <c r="L28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Júnior</v>
-      </c>
-      <c r="F28" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="M28" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>1870.2</v>
-      </c>
-      <c r="G28" s="3">
+        <v>168.31800000000001</v>
+      </c>
+      <c r="N28" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>1701.8820000000001</v>
+      </c>
+      <c r="O28" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>8.5009090909090919</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
+        <v>isento</v>
+      </c>
+      <c r="P28" s="3">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
-      <c r="J28" s="3">
-        <v>0</v>
-      </c>
-      <c r="K28" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>1870.2</v>
-      </c>
-      <c r="L28" s="13">
-        <f ca="1">VLOOKUP(K28,inss,2)</f>
-        <v>0.09</v>
-      </c>
-      <c r="M28" s="5">
-        <f ca="1">IF(L28="Teto",900.7,F28*L28)</f>
-        <v>168.31800000000001</v>
-      </c>
-      <c r="N28" s="5">
-        <f t="shared" ca="1" si="5"/>
+      <c r="Q28" s="5">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="5">
+        <f t="shared" ca="1" si="11"/>
         <v>1701.8820000000001</v>
       </c>
-      <c r="O28" s="13" t="str">
-        <f ca="1">VLOOKUP(N28,irrf,2)</f>
-        <v>isento</v>
-      </c>
-      <c r="P28" s="3">
-        <f ca="1">VLOOKUP(N28,irrf,3)</f>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="5">
-        <f t="shared" ca="1" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R28" s="5">
-        <f t="shared" ca="1" si="7"/>
-        <v>1701.8820000000001</v>
-      </c>
       <c r="S28" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>136.15056000000001</v>
       </c>
     </row>
@@ -2992,61 +2992,61 @@
         <v>47</v>
       </c>
       <c r="E29" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Pleno</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2431.2600000000002</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>11.051181818181819</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2431.2600000000002</v>
+      </c>
+      <c r="L29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Pleno</v>
-      </c>
-      <c r="F29" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M29" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2431.2600000000002</v>
-      </c>
-      <c r="G29" s="3">
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N29" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2139.5088000000001</v>
+      </c>
+      <c r="O29" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>11.051181818181819</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P29" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="3">
-        <v>0</v>
-      </c>
-      <c r="K29" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2431.2600000000002</v>
-      </c>
-      <c r="L29" s="13">
-        <f ca="1">VLOOKUP(K29,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M29" s="5">
-        <f ca="1">IF(L29="Teto",900.7,F29*L29)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N29" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2139.5088000000001</v>
-      </c>
-      <c r="O29" s="13">
-        <f ca="1">VLOOKUP(N29,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P29" s="3">
-        <f ca="1">VLOOKUP(N29,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q29" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>17.663159999999976</v>
       </c>
       <c r="R29" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2121.84564</v>
       </c>
       <c r="S29" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>171.16070400000001</v>
       </c>
     </row>
@@ -3064,61 +3064,61 @@
         <v>45</v>
       </c>
       <c r="E30" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2701.4</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>12.279090909090909</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="J30" s="3">
         <v>300</v>
       </c>
       <c r="K30" s="3">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="8"/>
         <v>3001.4</v>
       </c>
-      <c r="L30" s="13">
-        <f ca="1">VLOOKUP(K30,inss,2)</f>
+      <c r="L30" s="11">
+        <f t="shared" ca="1" si="0"/>
         <v>0.12</v>
       </c>
       <c r="M30" s="5">
-        <f ca="1">IF(L30="Teto",900.7,F30*L30)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>324.16800000000001</v>
       </c>
       <c r="N30" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="9"/>
         <v>2677.232</v>
       </c>
-      <c r="O30" s="13">
-        <f ca="1">VLOOKUP(N30,irrf,2)</f>
+      <c r="O30" s="11">
+        <f t="shared" ca="1" si="2"/>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="P30" s="3">
-        <f ca="1">VLOOKUP(N30,irrf,3)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>142.80000000000001</v>
       </c>
       <c r="Q30" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>57.992399999999975</v>
       </c>
       <c r="R30" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2619.2395999999999</v>
       </c>
       <c r="S30" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>214.17856</v>
       </c>
     </row>
@@ -3136,61 +3136,61 @@
         <v>44</v>
       </c>
       <c r="E31" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2431.2600000000002</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>11.051181818181819</v>
       </c>
       <c r="H31">
         <v>3</v>
       </c>
       <c r="I31" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>49.730318181818191</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+      <c r="K31" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2480.9903181818186</v>
+      </c>
+      <c r="L31" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="M31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N31" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2189.2391181818184</v>
+      </c>
+      <c r="O31" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P31" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>49.730318181818191</v>
-      </c>
-      <c r="J31" s="3">
-        <v>0</v>
-      </c>
-      <c r="K31" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2480.9903181818186</v>
-      </c>
-      <c r="L31" s="13">
-        <f ca="1">VLOOKUP(K31,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M31" s="5">
-        <f ca="1">IF(L31="Teto",900.7,F31*L31)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N31" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2189.2391181818184</v>
-      </c>
-      <c r="O31" s="13">
-        <f ca="1">VLOOKUP(N31,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P31" s="3">
-        <f ca="1">VLOOKUP(N31,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q31" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>21.392933863636358</v>
       </c>
       <c r="R31" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2167.8461843181822</v>
       </c>
       <c r="S31" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>175.13912945454547</v>
       </c>
     </row>
@@ -3208,61 +3208,61 @@
         <v>44</v>
       </c>
       <c r="E32" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2431.2600000000002</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>11.051181818181819</v>
       </c>
       <c r="H32">
         <v>5</v>
       </c>
       <c r="I32" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>82.883863636363643</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2514.1438636363637</v>
+      </c>
+      <c r="L32" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="M32" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N32" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2222.3926636363635</v>
+      </c>
+      <c r="O32" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P32" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>82.883863636363643</v>
-      </c>
-      <c r="J32" s="3">
-        <v>0</v>
-      </c>
-      <c r="K32" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2514.1438636363637</v>
-      </c>
-      <c r="L32" s="13">
-        <f ca="1">VLOOKUP(K32,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M32" s="5">
-        <f ca="1">IF(L32="Teto",900.7,F32*L32)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N32" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2222.3926636363635</v>
-      </c>
-      <c r="O32" s="13">
-        <f ca="1">VLOOKUP(N32,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P32" s="3">
-        <f ca="1">VLOOKUP(N32,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q32" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>23.879449772727241</v>
       </c>
       <c r="R32" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2198.5132138636363</v>
       </c>
       <c r="S32" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>177.79141309090909</v>
       </c>
     </row>
@@ -3280,58 +3280,58 @@
         <v>48</v>
       </c>
       <c r="E33" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Pleno</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2701.4</v>
+      </c>
+      <c r="G33" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>12.279090909090909</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0</v>
+      </c>
+      <c r="K33" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2701.4</v>
+      </c>
+      <c r="L33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Pleno</v>
-      </c>
-      <c r="F33" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M33" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2701.4</v>
-      </c>
-      <c r="G33" s="3">
+        <v>324.16800000000001</v>
+      </c>
+      <c r="N33" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2377.232</v>
+      </c>
+      <c r="O33" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>12.279090909090909</v>
-      </c>
-      <c r="I33" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P33" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="3">
-        <v>0</v>
-      </c>
-      <c r="K33" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2701.4</v>
-      </c>
-      <c r="L33" s="13">
-        <f ca="1">VLOOKUP(K33,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M33" s="5">
-        <f ca="1">IF(L33="Teto",900.7,F33*L33)</f>
-        <v>324.16800000000001</v>
-      </c>
-      <c r="N33" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2377.232</v>
-      </c>
-      <c r="O33" s="13">
-        <f ca="1">VLOOKUP(N33,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P33" s="3">
-        <f ca="1">VLOOKUP(N33,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q33" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>35.492399999999975</v>
       </c>
       <c r="R33" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2341.7395999999999</v>
       </c>
       <c r="S33" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>190.17856</v>
       </c>
     </row>
@@ -3349,61 +3349,61 @@
         <v>49</v>
       </c>
       <c r="E34" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2431.2600000000002</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>11.051181818181819</v>
       </c>
       <c r="H34">
         <v>10</v>
       </c>
       <c r="I34" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>165.76772727272729</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2597.0277272727276</v>
+      </c>
+      <c r="L34" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="M34" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N34" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2305.2765272727274</v>
+      </c>
+      <c r="O34" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P34" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>165.76772727272729</v>
-      </c>
-      <c r="J34" s="3">
-        <v>0</v>
-      </c>
-      <c r="K34" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2597.0277272727276</v>
-      </c>
-      <c r="L34" s="13">
-        <f ca="1">VLOOKUP(K34,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M34" s="5">
-        <f ca="1">IF(L34="Teto",900.7,F34*L34)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N34" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2305.2765272727274</v>
-      </c>
-      <c r="O34" s="13">
-        <f ca="1">VLOOKUP(N34,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P34" s="3">
-        <f ca="1">VLOOKUP(N34,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q34" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>30.095739545454535</v>
       </c>
       <c r="R34" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2275.1807877272731</v>
       </c>
       <c r="S34" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>184.4221221818182</v>
       </c>
     </row>
@@ -3421,61 +3421,61 @@
         <v>48</v>
       </c>
       <c r="E35" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Júnior</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2078</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>9.4454545454545453</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0</v>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2078</v>
+      </c>
+      <c r="L35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Júnior</v>
-      </c>
-      <c r="F35" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="M35" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2078</v>
-      </c>
-      <c r="G35" s="3">
+        <v>187.01999999999998</v>
+      </c>
+      <c r="N35" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>1890.98</v>
+      </c>
+      <c r="O35" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>9.4454545454545453</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35" s="3">
+        <v>isento</v>
+      </c>
+      <c r="P35" s="3">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
-      <c r="J35" s="3">
-        <v>0</v>
-      </c>
-      <c r="K35" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2078</v>
-      </c>
-      <c r="L35" s="13">
-        <f ca="1">VLOOKUP(K35,inss,2)</f>
-        <v>0.09</v>
-      </c>
-      <c r="M35" s="5">
-        <f ca="1">IF(L35="Teto",900.7,F35*L35)</f>
-        <v>187.01999999999998</v>
-      </c>
-      <c r="N35" s="5">
-        <f t="shared" ca="1" si="5"/>
+      <c r="Q35" s="5">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R35" s="5">
+        <f t="shared" ca="1" si="11"/>
         <v>1890.98</v>
       </c>
-      <c r="O35" s="13" t="str">
-        <f ca="1">VLOOKUP(N35,irrf,2)</f>
-        <v>isento</v>
-      </c>
-      <c r="P35" s="3">
-        <f ca="1">VLOOKUP(N35,irrf,3)</f>
-        <v>0</v>
-      </c>
-      <c r="Q35" s="5">
-        <f t="shared" ca="1" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R35" s="5">
-        <f t="shared" ca="1" si="7"/>
-        <v>1890.98</v>
-      </c>
       <c r="S35" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>151.2784</v>
       </c>
     </row>
@@ -3493,61 +3493,61 @@
         <v>42</v>
       </c>
       <c r="E36" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Pleno</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>3376.75</v>
+      </c>
+      <c r="G36" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>15.348863636363637</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+      <c r="K36" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>3376.75</v>
+      </c>
+      <c r="L36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Pleno</v>
-      </c>
-      <c r="F36" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M36" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>3376.75</v>
-      </c>
-      <c r="G36" s="3">
+        <v>472.74500000000006</v>
+      </c>
+      <c r="N36" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2904.0050000000001</v>
+      </c>
+      <c r="O36" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>15.348863636363637</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="P36" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="3">
-        <v>0</v>
-      </c>
-      <c r="K36" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3376.75</v>
-      </c>
-      <c r="L36" s="13">
-        <f ca="1">VLOOKUP(K36,inss,2)</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M36" s="5">
-        <f ca="1">IF(L36="Teto",900.7,F36*L36)</f>
-        <v>472.74500000000006</v>
-      </c>
-      <c r="N36" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2904.0050000000001</v>
-      </c>
-      <c r="O36" s="13">
-        <f ca="1">VLOOKUP(N36,irrf,2)</f>
-        <v>0.15</v>
-      </c>
-      <c r="P36" s="3">
-        <f ca="1">VLOOKUP(N36,irrf,3)</f>
         <v>354.8</v>
       </c>
       <c r="Q36" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>80.800749999999994</v>
       </c>
       <c r="R36" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2823.2042500000002</v>
       </c>
       <c r="S36" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>232.32040000000001</v>
       </c>
     </row>
@@ -3565,61 +3565,61 @@
         <v>46</v>
       </c>
       <c r="E37" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Senior</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2992.3199999999997</v>
+      </c>
+      <c r="G37" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>13.601454545454544</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2992.3199999999997</v>
+      </c>
+      <c r="L37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Senior</v>
-      </c>
-      <c r="F37" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M37" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2992.3199999999997</v>
-      </c>
-      <c r="G37" s="3">
+        <v>359.07839999999993</v>
+      </c>
+      <c r="N37" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2633.2415999999998</v>
+      </c>
+      <c r="O37" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>13.601454545454544</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P37" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="3">
-        <v>0</v>
-      </c>
-      <c r="K37" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2992.3199999999997</v>
-      </c>
-      <c r="L37" s="13">
-        <f ca="1">VLOOKUP(K37,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M37" s="5">
-        <f ca="1">IF(L37="Teto",900.7,F37*L37)</f>
-        <v>359.07839999999993</v>
-      </c>
-      <c r="N37" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2633.2415999999998</v>
-      </c>
-      <c r="O37" s="13">
-        <f ca="1">VLOOKUP(N37,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P37" s="3">
-        <f ca="1">VLOOKUP(N37,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q37" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>54.693119999999965</v>
       </c>
       <c r="R37" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2578.5484799999999</v>
       </c>
       <c r="S37" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>210.65932799999999</v>
       </c>
     </row>
@@ -3637,61 +3637,61 @@
         <v>46</v>
       </c>
       <c r="E38" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Pleno</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2431.2600000000002</v>
+      </c>
+      <c r="G38" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>11.051181818181819</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0</v>
+      </c>
+      <c r="K38" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2431.2600000000002</v>
+      </c>
+      <c r="L38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Pleno</v>
-      </c>
-      <c r="F38" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M38" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2431.2600000000002</v>
-      </c>
-      <c r="G38" s="3">
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N38" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2139.5088000000001</v>
+      </c>
+      <c r="O38" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>11.051181818181819</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P38" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="3">
-        <v>0</v>
-      </c>
-      <c r="K38" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2431.2600000000002</v>
-      </c>
-      <c r="L38" s="13">
-        <f ca="1">VLOOKUP(K38,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M38" s="5">
-        <f ca="1">IF(L38="Teto",900.7,F38*L38)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N38" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2139.5088000000001</v>
-      </c>
-      <c r="O38" s="13">
-        <f ca="1">VLOOKUP(N38,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P38" s="3">
-        <f ca="1">VLOOKUP(N38,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q38" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>17.663159999999976</v>
       </c>
       <c r="R38" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2121.84564</v>
       </c>
       <c r="S38" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>171.16070400000001</v>
       </c>
     </row>
@@ -3709,61 +3709,61 @@
         <v>43</v>
       </c>
       <c r="E39" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Pleno</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2026.05</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>9.2093181818181815</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0</v>
+      </c>
+      <c r="K39" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2026.05</v>
+      </c>
+      <c r="L39" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Pleno</v>
-      </c>
-      <c r="F39" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="M39" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2026.05</v>
-      </c>
-      <c r="G39" s="3">
+        <v>182.34449999999998</v>
+      </c>
+      <c r="N39" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>1843.7055</v>
+      </c>
+      <c r="O39" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>9.2093181818181815</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39" s="3">
+        <v>isento</v>
+      </c>
+      <c r="P39" s="3">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
-      <c r="J39" s="3">
-        <v>0</v>
-      </c>
-      <c r="K39" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2026.05</v>
-      </c>
-      <c r="L39" s="13">
-        <f ca="1">VLOOKUP(K39,inss,2)</f>
-        <v>0.09</v>
-      </c>
-      <c r="M39" s="5">
-        <f ca="1">IF(L39="Teto",900.7,F39*L39)</f>
-        <v>182.34449999999998</v>
-      </c>
-      <c r="N39" s="5">
-        <f t="shared" ca="1" si="5"/>
+      <c r="Q39" s="5">
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R39" s="5">
+        <f t="shared" ca="1" si="11"/>
         <v>1843.7055</v>
       </c>
-      <c r="O39" s="13" t="str">
-        <f ca="1">VLOOKUP(N39,irrf,2)</f>
-        <v>isento</v>
-      </c>
-      <c r="P39" s="3">
-        <f ca="1">VLOOKUP(N39,irrf,3)</f>
-        <v>0</v>
-      </c>
-      <c r="Q39" s="5">
-        <f t="shared" ca="1" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R39" s="5">
-        <f t="shared" ca="1" si="7"/>
-        <v>1843.7055</v>
-      </c>
       <c r="S39" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>147.49644000000001</v>
       </c>
     </row>
@@ -3781,61 +3781,61 @@
         <v>45</v>
       </c>
       <c r="E40" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Pleno</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2701.4</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>12.279090909090909</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0</v>
+      </c>
+      <c r="K40" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2701.4</v>
+      </c>
+      <c r="L40" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>Pleno</v>
-      </c>
-      <c r="F40" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="M40" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2701.4</v>
-      </c>
-      <c r="G40" s="3">
+        <v>324.16800000000001</v>
+      </c>
+      <c r="N40" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2377.232</v>
+      </c>
+      <c r="O40" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>12.279090909090909</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P40" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J40" s="3">
-        <v>0</v>
-      </c>
-      <c r="K40" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2701.4</v>
-      </c>
-      <c r="L40" s="13">
-        <f ca="1">VLOOKUP(K40,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M40" s="5">
-        <f ca="1">IF(L40="Teto",900.7,F40*L40)</f>
-        <v>324.16800000000001</v>
-      </c>
-      <c r="N40" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2377.232</v>
-      </c>
-      <c r="O40" s="13">
-        <f ca="1">VLOOKUP(N40,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P40" s="3">
-        <f ca="1">VLOOKUP(N40,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q40" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>35.492399999999975</v>
       </c>
       <c r="R40" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2341.7395999999999</v>
       </c>
       <c r="S40" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>190.17856</v>
       </c>
     </row>
@@ -3861,53 +3861,53 @@
         <v>4987.2</v>
       </c>
       <c r="G41" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>22.669090909090908</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>4987.2</v>
+      </c>
+      <c r="L41" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M41" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>698.20800000000008</v>
+      </c>
+      <c r="N41" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>4288.9920000000002</v>
+      </c>
+      <c r="O41" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>22.669090909090908</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41" s="3">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="P41" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J41" s="3">
-        <v>0</v>
-      </c>
-      <c r="K41" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>4987.2</v>
-      </c>
-      <c r="L41" s="13">
-        <f ca="1">VLOOKUP(K41,inss,2)</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M41" s="5">
-        <f ca="1">IF(L41="Teto",900.7,F41*L41)</f>
-        <v>698.20800000000008</v>
-      </c>
-      <c r="N41" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>4288.9920000000002</v>
-      </c>
-      <c r="O41" s="13">
-        <f ca="1">VLOOKUP(N41,irrf,2)</f>
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="P41" s="3">
-        <f ca="1">VLOOKUP(N41,irrf,3)</f>
         <v>636.13</v>
       </c>
       <c r="Q41" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>328.89320000000009</v>
       </c>
       <c r="R41" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>3960.0988000000002</v>
       </c>
       <c r="S41" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>343.11936000000003</v>
       </c>
     </row>
@@ -3925,61 +3925,61 @@
         <v>77</v>
       </c>
       <c r="E42" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Júnior</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1039</v>
       </c>
       <c r="G42" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>4.7227272727272727</v>
       </c>
       <c r="H42">
         <v>3</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="7"/>
         <v>21.252272727272725</v>
       </c>
       <c r="J42" s="3">
         <v>200</v>
       </c>
       <c r="K42" s="3">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="8"/>
         <v>1260.2522727272726</v>
       </c>
-      <c r="L42" s="13">
-        <f ca="1">VLOOKUP(K42,inss,2)</f>
+      <c r="L42" s="11">
+        <f t="shared" ca="1" si="0"/>
         <v>0.09</v>
       </c>
       <c r="M42" s="5">
-        <f ca="1">IF(L42="Teto",900.7,F42*L42)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>93.509999999999991</v>
       </c>
       <c r="N42" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="9"/>
         <v>1166.7422727272726</v>
       </c>
-      <c r="O42" s="13" t="str">
-        <f ca="1">VLOOKUP(N42,irrf,2)</f>
+      <c r="O42" s="11" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>isento</v>
       </c>
       <c r="P42" s="3">
-        <f ca="1">VLOOKUP(N42,irrf,3)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="Q42" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
       <c r="R42" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>1166.7422727272726</v>
       </c>
       <c r="S42" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>93.339381818181806</v>
       </c>
     </row>
@@ -3997,61 +3997,61 @@
         <v>47</v>
       </c>
       <c r="E43" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>Pleno</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2431.2600000000002</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="6"/>
         <v>11.051181818181819</v>
       </c>
       <c r="H43">
         <v>2</v>
       </c>
       <c r="I43" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>33.153545454545458</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0</v>
+      </c>
+      <c r="K43" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>2464.4135454545458</v>
+      </c>
+      <c r="L43" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="M43" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>291.75120000000004</v>
+      </c>
+      <c r="N43" s="5">
+        <f t="shared" ca="1" si="9"/>
+        <v>2172.6623454545456</v>
+      </c>
+      <c r="O43" s="11">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="P43" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>33.153545454545458</v>
-      </c>
-      <c r="J43" s="3">
-        <v>0</v>
-      </c>
-      <c r="K43" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2464.4135454545458</v>
-      </c>
-      <c r="L43" s="13">
-        <f ca="1">VLOOKUP(K43,inss,2)</f>
-        <v>0.12</v>
-      </c>
-      <c r="M43" s="5">
-        <f ca="1">IF(L43="Teto",900.7,F43*L43)</f>
-        <v>291.75120000000004</v>
-      </c>
-      <c r="N43" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>2172.6623454545456</v>
-      </c>
-      <c r="O43" s="13">
-        <f ca="1">VLOOKUP(N43,irrf,2)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="P43" s="3">
-        <f ca="1">VLOOKUP(N43,irrf,3)</f>
         <v>142.80000000000001</v>
       </c>
       <c r="Q43" s="5">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="13"/>
         <v>20.149675909090917</v>
       </c>
       <c r="R43" s="5">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>2152.5126695454546</v>
       </c>
       <c r="S43" s="5">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="12"/>
         <v>173.81298763636366</v>
       </c>
     </row>
@@ -4065,42 +4065,42 @@
       </c>
       <c r="G44" s="5"/>
       <c r="H44">
-        <f t="shared" ref="G44:S44" si="10">SUM(H7:H43)</f>
+        <f t="shared" ref="H44:S44" si="14">SUM(H7:H43)</f>
         <v>111</v>
       </c>
       <c r="I44" s="5">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="14"/>
         <v>2219.4925909090907</v>
       </c>
       <c r="J44" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1200</v>
       </c>
       <c r="K44" s="5">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="14"/>
         <v>101778.73259090907</v>
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="5">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="14"/>
         <v>11588.581300000003</v>
       </c>
       <c r="N44" s="5">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="14"/>
         <v>90190.151290909082</v>
       </c>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
       <c r="Q44" s="5">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="14"/>
         <v>2657.7712627272726</v>
       </c>
       <c r="R44" s="5">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="14"/>
         <v>87532.380028181797</v>
       </c>
       <c r="S44" s="5">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="14"/>
         <v>7215.2121032727273</v>
       </c>
     </row>

</xml_diff>